<commit_message>
Ft: addUsersValidation email is required input
</commit_message>
<xml_diff>
--- a/tests/mockData/addUsersDataInvalidInputs.xlsx
+++ b/tests/mockData/addUsersDataInvalidInputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Documents/Github/v9-bears-team-21/tests/mockData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{17413F3C-2627-3B4E-A0F0-52836076E546}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7012292A-B1BD-984E-A516-ECD248F16DCB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{B8C56E69-2D29-2E4A-B29E-E9524DFE2F7E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>first_name</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>James2323</t>
+  </si>
+  <si>
+    <t>james@gmail.com</t>
+  </si>
+  <si>
+    <t>jack@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -88,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +106,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,16 +136,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,7 +464,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,6 +517,9 @@
       <c r="F2">
         <v>232323</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -537,8 +557,15 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{1442F2EF-BE07-0B46-8AC6-BA90A1F9BB80}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{D6CE0463-BA11-AC41-BBBE-4E0B3022BAFC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>